<commit_message>
notes on shrubs a few updates to coefficients file
</commit_message>
<xml_diff>
--- a/fates-figs/mn-model-coeff.xlsx
+++ b/fates-figs/mn-model-coeff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/My Drive/My_Drive_Cloud/Drive-Projects/Pepperwood/Pepperwood_git_projects/ppw_working/fates-figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D7D66E6-0A7A-9645-9282-AAB080C42AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF13260-315F-5745-A4CA-455E4F1E2198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1920" windowWidth="23900" windowHeight="14980" xr2:uid="{78A4CAE7-FD12-1B43-9FA7-1C1EA82D058E}"/>
+    <workbookView xWindow="6640" yWindow="1240" windowWidth="31520" windowHeight="19740" xr2:uid="{78A4CAE7-FD12-1B43-9FA7-1C1EA82D058E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>Factors</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>ARCMAN</t>
+  </si>
+  <si>
+    <t>Interactions</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -460,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5748C2-30C0-1949-96F5-48E69BC89B38}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:M14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,15 +478,15 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -493,35 +499,38 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>15</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>16</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -537,64 +546,67 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="G3">
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>-2.2901199054244001</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>0.26649547406899099</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>-9.3036919489910705E-2</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>-0.50582873624093105</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>2.37177466534843</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>2.1595462083299202</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>3.0217158801241601</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>-0.87746460180236996</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>2.6723142290469002</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>1.4666318467342201</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>4.50899992327993</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>5.6838578639035298</v>
       </c>
-      <c r="L4" s="1">
+      <c r="M4" s="1">
         <v>-4.8384672592525</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>-6.19933694707104</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>-8.2638004909243907</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>0.25001202596704603</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -610,67 +622,70 @@
       <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" t="s">
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G7">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>1.9596594623533199</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>1.6353702798729799</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>4.74402762567086</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>5.7112054826467604</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>-4.9192930092215903</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>-6.3399836316356097</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>-9.8148620629507306</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H8" s="1"/>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -686,80 +701,83 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G10">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H10">
         <v>1</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>-0.23636015985318901</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>1.5305412178759199</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>1.2297498488369301</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>-1.76703206490466</v>
       </c>
-      <c r="L10" s="1">
+      <c r="M10" s="1">
         <v>-1.3211215069773701</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>1.62259837482605</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G11">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H11">
         <v>2</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>2.6666071694862201</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>-3.4764301475002699</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>-3.7454234518255798</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>-1.3423419007444</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>-1.55974374350927</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>0.46883724051103698</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="H12" s="1"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -775,35 +793,38 @@
       <c r="E13" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G14">
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H14">
         <v>2</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>1.4661895050482701</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>-11.552334063799099</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>-2.8524549519965201</v>
       </c>
-      <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
models updated. I don't understand common hardwood results
</commit_message>
<xml_diff>
--- a/fates-figs/mn-model-coeff.xlsx
+++ b/fates-figs/mn-model-coeff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/My Drive/My_Drive_Cloud/Drive-Projects/Pepperwood/Pepperwood_git_projects/ppw_working/fates-figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF13260-315F-5745-A4CA-455E4F1E2198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9C3F71-F87C-3540-B5FB-74357DC9383C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6640" yWindow="1240" windowWidth="31520" windowHeight="19740" xr2:uid="{78A4CAE7-FD12-1B43-9FA7-1C1EA82D058E}"/>
+    <workbookView xWindow="2280" yWindow="1920" windowWidth="23900" windowHeight="14980" xr2:uid="{78A4CAE7-FD12-1B43-9FA7-1C1EA82D058E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>Factors</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Common hardwoods</t>
   </si>
   <si>
-    <t>Fate</t>
-  </si>
-  <si>
     <t>Coefficients</t>
   </si>
   <si>
@@ -114,6 +111,45 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Fire:Size; Fire:Northness</t>
+  </si>
+  <si>
+    <t>fsCat1:northness</t>
+  </si>
+  <si>
+    <t>fsCat2:northness</t>
+  </si>
+  <si>
+    <t>fsCat3:northness</t>
+  </si>
+  <si>
+    <t>TSizeCatTR1:fsCat1</t>
+  </si>
+  <si>
+    <t>TSizeCatTR2:fsCat1</t>
+  </si>
+  <si>
+    <t>TSizeCatTR3:fsCat1</t>
+  </si>
+  <si>
+    <t>TSizeCatTR1:fsCat2</t>
+  </si>
+  <si>
+    <t>TSizeCatTR2:fsCat2</t>
+  </si>
+  <si>
+    <t>TSizeCatTR3:fsCat2</t>
+  </si>
+  <si>
+    <t>TSizeCatTR1:fsCat3</t>
+  </si>
+  <si>
+    <t>TSizeCatTR2:fsCat3</t>
+  </si>
+  <si>
+    <t>TSizeCatTR3:fsCat3</t>
   </si>
 </sst>
 </file>
@@ -466,27 +502,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5748C2-30C0-1949-96F5-48E69BC89B38}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -500,159 +537,263 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="P2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>-2.2901199054244001</v>
+        <v>-48.745599769925597</v>
       </c>
       <c r="J3" s="1">
-        <v>0.26649547406899099</v>
+        <v>-11.9116843011664</v>
       </c>
       <c r="K3" s="1">
-        <v>-9.3036919489910705E-2</v>
+        <v>-28.111517637552598</v>
       </c>
       <c r="L3" s="1">
-        <v>-0.50582873624093105</v>
+        <v>2.4617176961584302</v>
       </c>
       <c r="M3" s="1">
-        <v>2.37177466534843</v>
+        <v>49.121575488957497</v>
       </c>
       <c r="N3" s="1">
-        <v>2.1595462083299202</v>
+        <v>48.662570208942</v>
       </c>
       <c r="O3" s="1">
-        <v>3.0217158801241601</v>
+        <v>48.968179831545399</v>
       </c>
       <c r="P3" s="1">
-        <v>-0.87746460180236996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H4">
+        <v>113.149905651034</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>-115.37580436776901</v>
+      </c>
+      <c r="R3" s="1">
+        <v>-112.732880524892</v>
+      </c>
+      <c r="S3" s="1">
+        <v>-113.430889607518</v>
+      </c>
+      <c r="T3" s="1">
+        <v>12.3968233494017</v>
+      </c>
+      <c r="U3" s="1">
+        <v>26.286124676134101</v>
+      </c>
+      <c r="V3" s="1">
+        <v>-4.6184443294156399</v>
+      </c>
+      <c r="W3" s="1">
+        <v>11.932848627102301</v>
+      </c>
+      <c r="X3" s="1">
+        <v>28.257116276785499</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>-3.4364280206032101</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>12.651242700557299</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>29.4046904535987</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>-1.3739425637656699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
         <v>2</v>
       </c>
       <c r="I4" s="1">
-        <v>2.6723142290469002</v>
+        <v>3.5886078648774502</v>
       </c>
       <c r="J4" s="1">
-        <v>1.4666318467342201</v>
+        <v>0.40963981415978101</v>
       </c>
       <c r="K4" s="1">
-        <v>4.50899992327993</v>
+        <v>-1.43522993973628</v>
       </c>
       <c r="L4" s="1">
-        <v>5.6838578639035298</v>
+        <v>-0.55337346475902405</v>
       </c>
       <c r="M4" s="1">
-        <v>-4.8384672592525</v>
+        <v>-5.5793283272545402</v>
       </c>
       <c r="N4" s="1">
-        <v>-6.19933694707104</v>
+        <v>-78.283956735203205</v>
       </c>
       <c r="O4" s="1">
-        <v>-8.2638004909243907</v>
+        <v>-93.330840633817701</v>
       </c>
       <c r="P4" s="1">
-        <v>0.25001202596704603</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+        <v>-1.5972560547421299</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0.88597935747399204</v>
+      </c>
+      <c r="R4" s="1">
+        <v>3.1772367954099199</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1.14593496669057</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1.41616236689124</v>
+      </c>
+      <c r="U4" s="1">
+        <v>5.4505343206587904</v>
+      </c>
+      <c r="V4" s="1">
+        <v>5.5066099172658696</v>
+      </c>
+      <c r="W4" s="1">
+        <v>71.4584686551148</v>
+      </c>
+      <c r="X4" s="1">
+        <v>77.430876355669596</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>77.560921334759399</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>30.793697972078199</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>89.070122043649306</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>91.434914507301698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H7">
-        <v>2</v>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H7" s="1">
+        <v>1</v>
       </c>
       <c r="I7" s="1">
         <v>1.9596594623533199</v>
@@ -676,7 +817,7 @@
         <v>-9.8148620629507306</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -685,46 +826,47 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="J9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="L9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H10">
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H10" s="1">
         <v>1</v>
       </c>
       <c r="I10" s="1">
@@ -746,8 +888,8 @@
         <v>1.62259837482605</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H11">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H11" s="1">
         <v>2</v>
       </c>
       <c r="I11" s="1">
@@ -769,7 +911,7 @@
         <v>0.46883724051103698</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -777,41 +919,42 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="J13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H14">
-        <v>2</v>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="H14" s="1">
+        <v>1</v>
       </c>
       <c r="I14" s="1">
         <v>1.4661895050482701</v>

</xml_diff>